<commit_message>
complete update db to ex
</commit_message>
<xml_diff>
--- a/recommendApi/media/jobDbData1.xlsx
+++ b/recommendApi/media/jobDbData1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,12 +736,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>639134d66f6f2bd65dcbd8be</t>
+          <t>639145020f9362b03ae3d0b8</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ứng_viên vui_lòng gửi cv tiếng tiếng việt process nhanh_chóng sinh_viên ngành khoa_học máy_tính phần_mềm trường cao_đẳng đại_học có_thể tham_gia thực_tập công_ty tương_đương hiểu_biết tìm_hiểu lập_trình website ngôn_ngữ php mảng back end phát_triển web php php mysql php famework chúng_tôi framework tùy yêu_cầu khách_hàng codeigniter cakephp zend javascript js frameworks jquery angularjs vuejs db mysql thiết_kế database giao_tiếp chủ_động công_việc đam_mê phát_triển phần_mềm kỹ_năng làm_việc hòa tư_duy logic tạođiều bắt_buộc sinh_viên thực_tập công_ty trở_thành nhân_viên chính_thức kết_thúc thời_gian thực_tập công_ty đánh_giá sinh_viên năng_lực sinh_viên trở_thành nhân_viên chính_thức có_thể chính_thức tốt_nghiệp đào_tạo phát_triển hệ_thống web thực_tế phát_triển phần_mềm ngôn_ngữ php kỹ_thuật nắm_bắt nghiệp_vụ phân_tích phát_triển hệ_thống web kỹ_sư việt_nam nhật thực_hiện công_việc liên_quan yêu_cầu tythực php</t>
+          <t>kinh_nghiệm làm_việc reactjs kinh_nghiệm web services giỏi lập_trình chức_năng mẫu thiết_kế làm_việc html css javascript json tiếng đọc chú_trọng chi_tiết tư_duy phục_vụ khách_hàng chủ_động tích_cực khả_năng làm_việc độc_lập vàtrong kiến_thức lĩnh_vực giáo_dục cộng thực_hiện phương_pháp scrum agile phát_triển ứng_dụng web bao_gồm trang_web tương táchệ thống quản_lý khách_hàng chính_phủ việt nam làm_việc reactjs reduxsaga html css javascript môi_trường máy_chủ firebase nodejs vps có_thể tùy_chọn chỉ_định làm_việc ứng_dụng thiết_bị di_độngdự án quan_tâm react native làm_việc laptop nhânfrontend developer reactjs</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>639145020f9362b03ae3d0b8</t>
+          <t>639145e90f9362b03ae3d0be</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>kinh_nghiệm làm_việc reactjs kinh_nghiệm web services giỏi lập_trình chức_năng mẫu thiết_kế làm_việc html css javascript json tiếng đọc chú_trọng chi_tiết tư_duy phục_vụ khách_hàng chủ_động tích_cực khả_năng làm_việc độc_lập vàtrong kiến_thức lĩnh_vực giáo_dục cộng thực_hiện phương_pháp scrum agile phát_triển ứng_dụng web bao_gồm trang_web tương táchệ thống quản_lý khách_hàng chính_phủ việt nam làm_việc reactjs reduxsaga html css javascript môi_trường máy_chủ firebase nodejs vps có_thể tùy_chọn chỉ_định làm_việc ứng_dụng thiết_bị di_độngdự án quan_tâm react native làm_việc laptop nhânfrontend developer reactjs</t>
+          <t>kinh_nghiệm phát_triển ứng_dụng web ít_nhất kinh_nghiệm reactjs nextjs cam_kết chất_lượng tiếp_cận công_việc kỹ_lưỡng làm_việc tin_cậy năng_động nhiệt_tình khả_năng quản_lý điều_phối dự_án lương thoải_mái kiến thức đam_mê công_nghệ mong_muốn nâng năng_lực xem_xét yêu_cầu nghiệp_vụ làm_việc thành_viên thực_hiện phân_tích yêu_cầu kỹ_thuật viết mã rõ_ràng sạch_sẽ khả_năng kiểm_soát lỗi phối_hợp bộ_phận lỗi có_thể khắc_phục nhanh_chóng đóng_góp_ý_kiến ứng_dụng sử_dụng phát_triển bảo_trì ứng_dụng reactjs nextjs html js css đảm_bảo thời_gian chất_lượng sản phẩmjunior reactjs</t>
         </is>
       </c>
     </row>
@@ -766,12 +766,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>639145e90f9362b03ae3d0be</t>
+          <t>639147560f9362b03ae3d0ca</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>kinh_nghiệm phát_triển ứng_dụng web ít_nhất kinh_nghiệm reactjs nextjs cam_kết chất_lượng tiếp_cận công_việc kỹ_lưỡng làm_việc tin_cậy năng_động nhiệt_tình khả_năng quản_lý điều_phối dự_án lương thoải_mái kiến thức đam_mê công_nghệ mong_muốn nâng năng_lực xem_xét yêu_cầu nghiệp_vụ làm_việc thành_viên thực_hiện phân_tích yêu_cầu kỹ_thuật viết mã rõ_ràng sạch_sẽ khả_năng kiểm_soát lỗi phối_hợp bộ_phận lỗi có_thể khắc_phục nhanh_chóng đóng_góp_ý_kiến ứng_dụng sử_dụng phát_triển bảo_trì ứng_dụng reactjs nextjs html js css đảm_bảo thời_gian chất_lượng sản phẩmjunior reactjs</t>
+          <t>ít_nhất phát_triển ứng_dụng nền_tảng android thành_thạo java kotlin kinh_nghiệm mẫu kiến_trúc ứng_dụng mvcmvpmvvm kinh_nghiệm kết_nối api google maps gcmfcm kinh_nghiệm thiết_kế ux ui application kiến_thức thiết_kế oop kiến_thức mẫu thiết_kế lợi_thế khả_năng làm_việc độc_lập nhómhợp tác chặt_chẽ bộ_phận liên_quan phát_triển ứng_dụng payoo nền_tảng android hỗ_trợ đối_tác tích_hợp sdk dự_án thúc_đẩy tính_năng cần_thiết phát_triển sản_phẩm phát_triển ý_tưởng ứng_dụng payoo tái kiến_trúc ứng_dụng payoo nền_tảng android duy_trì cải_thiện hiệu_suất sửa lỗi ứng_dụng tham_gia thảo_luận thết kế ứng_dụng phát_triển codeunitintergrationui tài_liệu thực_hiện dự_án thảo_luận quản_lý trực_tiếp ban giám đốcandroid developer</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>639147560f9362b03ae3d0ca</t>
+          <t>639147bc0f9362b03ae3d0d4</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ít_nhất phát_triển ứng_dụng nền_tảng android thành_thạo java kotlin kinh_nghiệm mẫu kiến_trúc ứng_dụng mvcmvpmvvm kinh_nghiệm kết_nối api google maps gcmfcm kinh_nghiệm thiết_kế ux ui application kiến_thức thiết_kế oop kiến_thức mẫu thiết_kế lợi_thế khả_năng làm_việc độc_lập nhómhợp tác chặt_chẽ bộ_phận liên_quan phát_triển ứng_dụng payoo nền_tảng android hỗ_trợ đối_tác tích_hợp sdk dự_án thúc_đẩy tính_năng cần_thiết phát_triển sản_phẩm phát_triển ý_tưởng ứng_dụng payoo tái kiến_trúc ứng_dụng payoo nền_tảng android duy_trì cải_thiện hiệu_suất sửa lỗi ứng_dụng tham_gia thảo_luận thết kế ứng_dụng phát_triển codeunitintergrationui tài_liệu thực_hiện dự_án thảo_luận quản_lý trực_tiếp ban giám đốcandroid developer</t>
+          <t>kinh_nghiệm phát_triển ứng_dụng di_động ngôn_ngữ swift object c ios java android flutter lợi_thế hiểu_biết kỹ_năng cơ_bản lập_trình hướng đối_tượng sử_dụng tool quản_lý source git svn khả_năng tự_quản_lý trách_nhiệm có_thể giao_tiếp làm_việc tham_gia phát_triển ứng_dụng mobile ios android hằng native react native flutter tập_trung hiệu_suất chất_lượng ứng_dụng hoàn_thiện trải nghiệm ux xây_dựng tối_ưu_hóa thông_số kỹ_thuật tiêu_chuẩn quá_trình phát_triển cải_thiện quy_trình phát_triển nghiên_cứu phân_tích giải_pháp kỹ_thuật đánh_giá giới_thiệu thúc_đẩy công_nghệ giải_quyết vấn_đề kỹ_thuật thực_hiện cụ_thể tham_gia xây_dựng nền_tảng có_thể đảm_trách vị_trí head of mobile team kỹ_năng kinh nghiệmlập viên mobile ios android</t>
         </is>
       </c>
     </row>
@@ -796,12 +796,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>639147bc0f9362b03ae3d0d4</t>
+          <t>639148520f9362b03ae3d0de</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>kinh_nghiệm phát_triển ứng_dụng di_động ngôn_ngữ swift object c ios java android flutter lợi_thế hiểu_biết kỹ_năng cơ_bản lập_trình hướng đối_tượng sử_dụng tool quản_lý source git svn khả_năng tự_quản_lý trách_nhiệm có_thể giao_tiếp làm_việc tham_gia phát_triển ứng_dụng mobile ios android hằng native react native flutter tập_trung hiệu_suất chất_lượng ứng_dụng hoàn_thiện trải nghiệm ux xây_dựng tối_ưu_hóa thông_số kỹ_thuật tiêu_chuẩn quá_trình phát_triển cải_thiện quy_trình phát_triển nghiên_cứu phân_tích giải_pháp kỹ_thuật đánh_giá giới_thiệu thúc_đẩy công_nghệ giải_quyết vấn_đề kỹ_thuật thực_hiện cụ_thể tham_gia xây_dựng nền_tảng có_thể đảm_trách vị_trí head of mobile team kỹ_năng kinh nghiệmlập viên mobile ios android</t>
+          <t>ít_nhất kinh_nghiệm phát_triển ios chuyên_nghiệp sử_dụng thành_thạo objectivec swift ios sdk rest api kinh_nghiệm ios framework core data core animation vv kinh_nghiệm lưu_trữ ngoại_tuyến phân_luồng điều_chỉnh hiệu_suất quen_thuộc api restful kết_nối ứng_dụng ios dịch_vụ backend kiến_thức công_nghệ web tiêu_chuẩn uiux hiểu_biết nguyên_tắc thiết_kế hướng_dẫn giao_diện apple kiến_thức phát_triển agilescrumkiểm định_hướng kiến_thức phát_triển backend kỹ_năng giao_tiếp tiếng thiết_kế xây_dựng ứng_dụng cao_cấp nền_tảng ios tương_tác khách_hàng cộng_tác đa chức_năng xác_định thiết_kế cung_cấp tính_năng wireframes thiết_kế phát_triển thử_nghiệm triển_khai ứng_dụng ios tiếp_tục sản_xuất phiên_bản ứng_dụng thiết_kế giải_pháp một_cách độc_lập mã kiểm_tra đơn_vị độ bền bao_gồm trường_hợp khả_năng sử_dụng độ tin_cậy làm_việc sửa lỗi cải_thiện hiệu_suất ứng_dụng hoạt_động hiệu_quả môi_trường lập_trình nhịp_độ thời_hạn hợp_tác lặp_đi lặp_lạimiddle ios developer</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>639148520f9362b03ae3d0de</t>
+          <t>63914f332e7bf4e4662d6375</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ít_nhất kinh_nghiệm phát_triển ios chuyên_nghiệp sử_dụng thành_thạo objectivec swift ios sdk rest api kinh_nghiệm ios framework core data core animation vv kinh_nghiệm lưu_trữ ngoại_tuyến phân_luồng điều_chỉnh hiệu_suất quen_thuộc api restful kết_nối ứng_dụng ios dịch_vụ backend kiến_thức công_nghệ web tiêu_chuẩn uiux hiểu_biết nguyên_tắc thiết_kế hướng_dẫn giao_diện apple kiến_thức phát_triển agilescrumkiểm định_hướng kiến_thức phát_triển backend kỹ_năng giao_tiếp tiếng thiết_kế xây_dựng ứng_dụng cao_cấp nền_tảng ios tương_tác khách_hàng cộng_tác đa chức_năng xác_định thiết_kế cung_cấp tính_năng wireframes thiết_kế phát_triển thử_nghiệm triển_khai ứng_dụng ios tiếp_tục sản_xuất phiên_bản ứng_dụng thiết_kế giải_pháp một_cách độc_lập mã kiểm_tra đơn_vị độ bền bao_gồm trường_hợp khả_năng sử_dụng độ tin_cậy làm_việc sửa lỗi cải_thiện hiệu_suất ứng_dụng hoạt_động hiệu_quả môi_trường lập_trình nhịp_độ thời_hạn hợp_tác lặp_đi lặp_lạimiddle ios developer</t>
+          <t>chăm_sóc giúp sinh_viên thay_đổi đường sự_nghiệp họkĩ năng giao_tiếp nói_chuyện sinh_viên hàng đánh_giá có_thể truyền_cảm_hứng hành_trình mớitính kiên_nhẫn học có_thể mới_mẻ đối_với họcó kinh_nghiệm làm_việc dữ_liệu ds ưu tiêncó kinh_nghiệm sqlbigquery python pandas seaborn matplotlibquen công_cụ trực_quan_hóa dữ_liệu tableau ưu_tiên powerbi google data studioquen học máy truyền_thống hồi tuyến tínhlogistic knn kmeans địnhai engineer</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>63914f332e7bf4e4662d6375</t>
+          <t>63914fb52e7bf4e4662d637f</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>chăm_sóc giúp sinh_viên thay_đổi đường sự_nghiệp họkĩ năng giao_tiếp nói_chuyện sinh_viên hàng đánh_giá có_thể truyền_cảm_hứng hành_trình mớitính kiên_nhẫn học có_thể mới_mẻ đối_với họcó kinh_nghiệm làm_việc dữ_liệu ds ưu tiêncó kinh_nghiệm sqlbigquery python pandas seaborn matplotlibquen công_cụ trực_quan_hóa dữ_liệu tableau ưu_tiên powerbi google data studioquen học máy truyền_thống hồi tuyến tínhlogistic knn kmeans địnhai engineer</t>
+          <t>ít_nhất kinh_nghiệm lĩnh_vực machine learning deep learning tham_gia ít_nhất project triển_khai thành_công sử_dụng sử_dụng thành_thạo ngôn_ngữ python go cc thành_thạo ít_nhất framework tensorflow keras pytorch sử_dụng thư_viện matplotlib numpy pandas ưu_tiên kinh_nghiệm sử_dụng opencv đọc tiếng kỹ_năng làm_việc tham_gia triển_khai dịch_vụ trí_tuệ nhân_tạo lĩnh_vực thị_giác máy_tính xử_lý ảnh xử_lý ngôn_ngữ tự_nhiên nghiên_cứu áp_dụng công_nghệ triển_khai bài_toán ứng_dụng ekyc chatbot scanextraction thông_tin giải_quyết bài_toán machine learning deep learning khácai engineer</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>63914fb52e7bf4e4662d637f</t>
+          <t>639150eb2e7bf4e4662d638f</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ít_nhất kinh_nghiệm lĩnh_vực machine learning deep learning tham_gia ít_nhất project triển_khai thành_công sử_dụng sử_dụng thành_thạo ngôn_ngữ python go cc thành_thạo ít_nhất framework tensorflow keras pytorch sử_dụng thư_viện matplotlib numpy pandas ưu_tiên kinh_nghiệm sử_dụng opencv đọc tiếng kỹ_năng làm_việc tham_gia triển_khai dịch_vụ trí_tuệ nhân_tạo lĩnh_vực thị_giác máy_tính xử_lý ảnh xử_lý ngôn_ngữ tự_nhiên nghiên_cứu áp_dụng công_nghệ triển_khai bài_toán ứng_dụng ekyc chatbot scanextraction thông_tin giải_quyết bài_toán machine learning deep learning khácai engineer</t>
+          <t>has years of experience working as an data developer scientist advance sql knowledge and experience working with rdbms as well as working farmiliarity with variety of databases and database engine experience building and optimizing data pipeline architectures and datasets in cloud build processes supporting data transformation data structures metadata dependency and workload management experience in data mining understanding of ml and operation research knowledge of sql and python it s plus if you known nodejs or javascript experience using bi tools and data frameworks good at math skillsdata warehouse data mining data pipeline google cloud platfarm pythontạo duy_trì kiến trúc đường_ống liệuxây dựng cơ_sở hạ_tầng cần_thiết trích chuyển_đổi tải dữ_liệu dữ_liệu công_nghệ sql gdpgiữ dữ_liệu phân_tách bảo_mật xuyên biên_giới quốc_gia thông_qua trung_tâm dữ_liệu gdpxây dựng công_cụ phân_tích tận_dụng đường truyền dữ_liệu cung_cấp sâu_sắc có_thể hành_động hiệu_quả hoạt_động chỉ_số_hiệu_suất kinh_doanh quan_trọng khácthực thu_thập tiền xử_lý phân_tích liệuáp_dụng ngôn_ngữ kỹ_thuật xây_dựng mô_hình giải_quyết vấn_đề kinh doanhxác dữ_liệu giá_trị tự_động hóa quy_trình thu thậpphân tích thông_tin khám_phá xu_hướng mô hìnhxây dựng mô_hình dự_đoán thuật_toán mltiến hành tiền xử_lý dữ_liệu cấu_trúc phi_cấu trúckết mô_hình thông_qua mô_hình hợpdata developer scientist</t>
         </is>
       </c>
     </row>
@@ -856,12 +856,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>639150eb2e7bf4e4662d638f</t>
+          <t>639152462e7bf4e4662d63a1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>has years of experience working as an data developer scientist advance sql knowledge and experience working with rdbms as well as working farmiliarity with variety of databases and database engine experience building and optimizing data pipeline architectures and datasets in cloud build processes supporting data transformation data structures metadata dependency and workload management experience in data mining understanding of ml and operation research knowledge of sql and python it s plus if you known nodejs or javascript experience using bi tools and data frameworks good at math skillsdata warehouse data mining data pipeline google cloud platfarm pythontạo duy_trì kiến trúc đường_ống liệuxây dựng cơ_sở hạ_tầng cần_thiết trích chuyển_đổi tải dữ_liệu dữ_liệu công_nghệ sql gdpgiữ dữ_liệu phân_tách bảo_mật xuyên biên_giới quốc_gia thông_qua trung_tâm dữ_liệu gdpxây dựng công_cụ phân_tích tận_dụng đường truyền dữ_liệu cung_cấp sâu_sắc có_thể hành_động hiệu_quả hoạt_động chỉ_số_hiệu_suất kinh_doanh quan_trọng khácthực thu_thập tiền xử_lý phân_tích liệuáp_dụng ngôn_ngữ kỹ_thuật xây_dựng mô_hình giải_quyết vấn_đề kinh doanhxác dữ_liệu giá_trị tự_động hóa quy_trình thu thậpphân tích thông_tin khám_phá xu_hướng mô hìnhxây dựng mô_hình dự_đoán thuật_toán mltiến hành tiền xử_lý dữ_liệu cấu_trúc phi_cấu trúckết mô_hình thông_qua mô_hình hợpdata developer scientist</t>
+          <t>nam tốt_nghiệp chuyên_ngành cơ_điện_tử công_nghệ thông_tin toán ứng_dụng khoa_học máy tínhhoặc chuyên_ngành liên_quan ngoại_ngữ tiếng đọc viết tiếng nhật ưu_tiên khả_năng lập_trình ngôn_ngữ c python nền_tảng cơ_bản xử_lý ảnh thị_giác máy_tính thuật_toán_học máy tiếp_xúc thư viên open cvtensorflowpytorch kiến_thức mô_hình thần_kinh nhân_tạo yolo autoencoder lợi_thế hiểu_biết plc lập_trình giao_tiếp máy_tính plc visual studio community pycharm community nhanh_nhẹn trung_thực tinh_thần trách_nhiệm hợp_tác team works giao_tiếp tự_tin cởi_mở áp_dụng thuật_toán xử_lý ảnh học máy học sâu bài_toán kiểm_tra ngoại sản_phẩm phân_tích hiệu_quả thuật_toán cải_tiến hệ thốngkỹ sư bộ_phận nghiên_cứu phát_triển</t>
         </is>
       </c>
     </row>
@@ -871,12 +871,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>639152462e7bf4e4662d63a1</t>
+          <t>639155242e7bf4e4662d63b1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>nam tốt_nghiệp chuyên_ngành cơ_điện_tử công_nghệ thông_tin toán ứng_dụng khoa_học máy tínhhoặc chuyên_ngành liên_quan ngoại_ngữ tiếng đọc viết tiếng nhật ưu_tiên khả_năng lập_trình ngôn_ngữ c python nền_tảng cơ_bản xử_lý ảnh thị_giác máy_tính thuật_toán_học máy tiếp_xúc thư viên open cvtensorflowpytorch kiến_thức mô_hình thần_kinh nhân_tạo yolo autoencoder lợi_thế hiểu_biết plc lập_trình giao_tiếp máy_tính plc visual studio community pycharm community nhanh_nhẹn trung_thực tinh_thần trách_nhiệm hợp_tác team works giao_tiếp tự_tin cởi_mở áp_dụng thuật_toán xử_lý ảnh học máy học sâu bài_toán kiểm_tra ngoại sản_phẩm phân_tích hiệu_quả thuật_toán cải_tiến hệ thốngkỹ sư bộ_phận nghiên_cứu phát_triển</t>
+          <t>cử_nhân khoa_học máy_tính kỹ_thuật lĩnh_vực liên_quan học máy toán_học thống_kê kinh_nghiệm thiết_lập xây_dựng kiến trúc dữ_liệu đường_ống triển_khai mô_hình môi_trường rõ_ràng kinh_nghiệm áp_dụng kỹ_thuật máy học giải_quyết vấn_đề kinh_doanh phức_tạp thông_số ảnh_hưởng hiệu_suất kinh_nghiệm phát_triển kế_hoạch thử_nghiệm phân_tích quy_trình mô_hình_hóa dữ_liệu sử_dụng đường cơ_sở vững_chắc khả_năng xác_định chính_xác quan_hệ nhân_quả thông_thạo thao_tác dữ_liệu dựa sql kinh_nghiệm chuyên_sâu sử_dụng ngôn_ngữ kịch_bản r python phân_tích dữ_liệu phát_triển mô_hình thống_kê phân_tích khám_phá hiểu_biết sâu_sắc phân khúc giúp thúc_đẩy doanh_nghiệp phát_triển khám_phá lĩnh_vực cơ_hội áp_dụng phương_pháp học máy phát_triển phát_triển thử_nghiệm cải_tiến chạy thử_nghiệm tính_toán tinh_chỉnh tham_số viết mã python r scala sql vv thao_tác phân_tích dữ_liệu data scientist</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>639155242e7bf4e4662d63b1</t>
+          <t>639155c42e7bf4e4662d63b5</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>cử_nhân khoa_học máy_tính kỹ_thuật lĩnh_vực liên_quan học máy toán_học thống_kê kinh_nghiệm thiết_lập xây_dựng kiến trúc dữ_liệu đường_ống triển_khai mô_hình môi_trường rõ_ràng kinh_nghiệm áp_dụng kỹ_thuật máy học giải_quyết vấn_đề kinh_doanh phức_tạp thông_số ảnh_hưởng hiệu_suất kinh_nghiệm phát_triển kế_hoạch thử_nghiệm phân_tích quy_trình mô_hình_hóa dữ_liệu sử_dụng đường cơ_sở vững_chắc khả_năng xác_định chính_xác quan_hệ nhân_quả thông_thạo thao_tác dữ_liệu dựa sql kinh_nghiệm chuyên_sâu sử_dụng ngôn_ngữ kịch_bản r python phân_tích dữ_liệu phát_triển mô_hình thống_kê phân_tích khám_phá hiểu_biết sâu_sắc phân khúc giúp thúc_đẩy doanh_nghiệp phát_triển khám_phá lĩnh_vực cơ_hội áp_dụng phương_pháp học máy phát_triển phát_triển thử_nghiệm cải_tiến chạy thử_nghiệm tính_toán tinh_chỉnh tham_số viết mã python r scala sql vv thao_tác phân_tích dữ_liệu data scientist</t>
+          <t>kiến_thức căn_bản data mining ml kiến_thức kinh_nghiệm sử_dụng spark etl with scala python hadoop ecosys kiến_thức kinh_nghiệm tối_ưu luồng xử_lý data landing zone working zone gold zone kỹ_thuật thiết_kế job tối_ưu dữ_liệu kỹ_thuật orchestration luồng job kiến_thức kinh_nghiệm db sql db oracle netezza mysql postgresql mariadb amazon aurona nosql db elasticsearch apache cassandra apache hbase google bigtale apache pinot graph db tigergraph amazon nepture memory db redis memcached kiến_thức kinh_nghiệm machine learning thoery keras tensorflow pytorch scikitlearn numpy pandas zeppline jupiter hub tham_gia quy_trình xây_dựng bảo_trì model elt data cleaning data analytic data building model testing model sharing with business for feedback deploying model visualization maintenance model educating business and teamschuyên giachuyên viên cao_cấp data engineer</t>
         </is>
       </c>
     </row>
@@ -901,12 +901,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>639155c42e7bf4e4662d63b5</t>
+          <t>639156872e7bf4e4662d63bb</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>kiến_thức căn_bản data mining ml kiến_thức kinh_nghiệm sử_dụng spark etl with scala python hadoop ecosys kiến_thức kinh_nghiệm tối_ưu luồng xử_lý data landing zone working zone gold zone kỹ_thuật thiết_kế job tối_ưu dữ_liệu kỹ_thuật orchestration luồng job kiến_thức kinh_nghiệm db sql db oracle netezza mysql postgresql mariadb amazon aurona nosql db elasticsearch apache cassandra apache hbase google bigtale apache pinot graph db tigergraph amazon nepture memory db redis memcached kiến_thức kinh_nghiệm machine learning thoery keras tensorflow pytorch scikitlearn numpy pandas zeppline jupiter hub tham_gia quy_trình xây_dựng bảo_trì model elt data cleaning data analytic data building model testing model sharing with business for feedback deploying model visualization maintenance model educating business and teamschuyên giachuyên viên cao_cấp data engineer</t>
+          <t>kinh_nghiệm làm_việc dịch_vụ web restful kiến_thức kinh_nghiệm rdbms sqlnosql kinh_nghiệm lập_trình ít_nhất javascript nodejs java spring c kinh_nghiệm môi_trường dựa linux khả_năng học_hỏi kinh_nghiệm sử_dụng công_cụ cộng_tác jira confluence kinh_nghiệm javamysqlelk cập_nhật xu_hướng thiết_kế công_nghệ cởi_mở thảo_luận thiết_kế đánh_giá mã kinh_nghiệm phát_triển dựa đám mây aws gcp kinh_nghiệm kiểm_soát phiên_bản git svn etc phát_triển dịch_vụ nền_tảng công_cụ vận_hành phát_hành game phát_triển restful api dựa nền_tảng liên_kết phát_triển phân_tích dữ_liệu đa_dạng xử_lý phân_phối dữ_liệu phát_triển dịch_vụ quản_lý thông_tin quản_lý_tài_khoản theo_dõi báo_cáo thống_kê cần_thiết phát_triển máy_chủ phụ_trợ giao_diện_tích_hợp nền_tảng cổng api hàng đợi nhắn phân_tán vv phát_triển hệ_thống xử_lý thời_gian game big databackend developer nodejs java c</t>
         </is>
       </c>
     </row>
@@ -916,12 +916,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>639156872e7bf4e4662d63bb</t>
+          <t>639159492e7bf4e4662d63dd</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>kinh_nghiệm làm_việc dịch_vụ web restful kiến_thức kinh_nghiệm rdbms sqlnosql kinh_nghiệm lập_trình ít_nhất javascript nodejs java spring c kinh_nghiệm môi_trường dựa linux khả_năng học_hỏi kinh_nghiệm sử_dụng công_cụ cộng_tác jira confluence kinh_nghiệm javamysqlelk cập_nhật xu_hướng thiết_kế công_nghệ cởi_mở thảo_luận thiết_kế đánh_giá mã kinh_nghiệm phát_triển dựa đám mây aws gcp kinh_nghiệm kiểm_soát phiên_bản git svn etc phát_triển dịch_vụ nền_tảng công_cụ vận_hành phát_hành game phát_triển restful api dựa nền_tảng liên_kết phát_triển phân_tích dữ_liệu đa_dạng xử_lý phân_phối dữ_liệu phát_triển dịch_vụ quản_lý thông_tin quản_lý_tài_khoản theo_dõi báo_cáo thống_kê cần_thiết phát_triển máy_chủ phụ_trợ giao_diện_tích_hợp nền_tảng cổng api hàng đợi nhắn phân_tán vv phát_triển hệ_thống xử_lý thời_gian game big databackend developer nodejs java c</t>
+          <t>kinh_nghiệm lập_trình unity kinh_nghiệm code dự_án game thẻ tướng game nhập_vai game kiến_thức chuyên_sâu lập_trình c java am_hiểu khía_cạnh phát_triển game bao_gồm ui animation sounds level design kinh_nghiệm tích_hợp firebase analytics fcm ít_nhất game code unity cá_nhân công_ty gửi kèm sản_phẩm cv ứng_tuyển kinh_nghiệm hyper casualcasual gamepuzzle game sử_dụng unity phát_triển mobile game phát_hành google play app store định_hướng thị_trường bắc mỹ tham_gia dự_án game code unity phần_mềm lập_trình phối_hợp thành_viên team hoàn_thiện tối_ưu game animation ui ux game developer unity developer</t>
         </is>
       </c>
     </row>
@@ -931,12 +931,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>639159492e7bf4e4662d63dd</t>
+          <t>639159c52e7bf4e4662d63e9</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>kinh_nghiệm lập_trình unity kinh_nghiệm code dự_án game thẻ tướng game nhập_vai game kiến_thức chuyên_sâu lập_trình c java am_hiểu khía_cạnh phát_triển game bao_gồm ui animation sounds level design kinh_nghiệm tích_hợp firebase analytics fcm ít_nhất game code unity cá_nhân công_ty gửi kèm sản_phẩm cv ứng_tuyển kinh_nghiệm hyper casualcasual gamepuzzle game sử_dụng unity phát_triển mobile game phát_hành google play app store định_hướng thị_trường bắc mỹ tham_gia dự_án game code unity phần_mềm lập_trình phối_hợp thành_viên team hoàn_thiện tối_ưu game animation ui ux game developer unity developer</t>
+          <t>tốt_nghiệp tốt_nghiệp chuyên_ngành cntt sử_dụng unity bắt_buộc nắm kiến_thức ngôn_ngữ lập_trình c c nắm vững kiến_thức cấu_trúc dữ_liệu giải_thuật thuật_toán nền_tảng oop khả_năng tư_duy học_hỏi kiến_thức game điện_thoại_di_động đọc tiếng dự_án game lợi_thế đào_tạo trở_thành nhân_viên chính_thức phối_hợp producer game designer artist phác_họa ý_tưởng xây_dựng trò_chơi prototype hướng_dẫn cài_đặt tính_năng phát_triển sản_phẩm gamegame development fresher</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>639159c52e7bf4e4662d63e9</t>
+          <t>63915a792e7bf4e4662d6401</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>tốt_nghiệp tốt_nghiệp chuyên_ngành cntt sử_dụng unity bắt_buộc nắm kiến_thức ngôn_ngữ lập_trình c c nắm vững kiến_thức cấu_trúc dữ_liệu giải_thuật thuật_toán nền_tảng oop khả_năng tư_duy học_hỏi kiến_thức game điện_thoại_di_động đọc tiếng dự_án game lợi_thế đào_tạo trở_thành nhân_viên chính_thức phối_hợp producer game designer artist phác_họa ý_tưởng xây_dựng trò_chơi prototype hướng_dẫn cài_đặt tính_năng phát_triển sản_phẩm gamegame development fresher</t>
+          <t>game ít_nhất kinh_nghiệm phát_triển trò_chơi khả_năng làm_việc khía_cạnh phát_triển ứng_dụng bao_gồm ui animation khả_năng leader mentor tốt_nghiệp cử_nhân khoa_học máy_tính liên_quan kiến_thức vững_chắc công_cụ phát_triển c hiểu_biết oop design patterns tư_duy logic chủ_động công_việc tinh_thần trách_nhiệm phát_triển mobile game nền_tảng unity phối_hợp thành_viên team hoàn_thiện tối_ưu game animation ui ux effect hỗ_trợ hướng_dẫn thành_viên junior nâng chuyên_môn tham_gia maintain game phát_hành prototype ý_tưởng game mớigame developer unity developer</t>
         </is>
       </c>
     </row>
@@ -961,25 +961,10 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>63915a792e7bf4e4662d6401</t>
+          <t>63915bf92e7bf4e4662d6415</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
-        <is>
-          <t>game ít_nhất kinh_nghiệm phát_triển trò_chơi khả_năng làm_việc khía_cạnh phát_triển ứng_dụng bao_gồm ui animation khả_năng leader mentor tốt_nghiệp cử_nhân khoa_học máy_tính liên_quan kiến_thức vững_chắc công_cụ phát_triển c hiểu_biết oop design patterns tư_duy logic chủ_động công_việc tinh_thần trách_nhiệm phát_triển mobile game nền_tảng unity phối_hợp thành_viên team hoàn_thiện tối_ưu game animation ui ux effect hỗ_trợ hướng_dẫn thành_viên junior nâng chuyên_môn tham_gia maintain game phát_hành prototype ý_tưởng game mớigame developer unity developer</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>63915bf92e7bf4e4662d6415</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
         <is>
           <t>tốt_nghiệp đại_học chuyên_ngành kỹ_thuật phần_mềm toán khoa_học máy_tính kinh_nghiệm làm_việc java core java frameworks spring framework spring boot kinh_nghiệm team lead kiến_thức kinh_nghiệm làm_việc nosql relational database microservices architecture software design principles unit and functional testing git and cicd lợi_thế hiểu_biết software logging and monitoring uml diagrams classsequence diagram lợi_thế quen_thuộc domain driven design devops and agile principles lợi_thế tham_gia xây_dựng platforms khả_năng scaling performance trải nghiệm khách_hàng nền_tảng phát_triển giải_quyết bài_toán data realtime recommendation realtime ab testing thiết_kế domain driven design triển_khai clean code unit test deployment đảm_bảo_an_toàn hệ_thống hỗ_trợ tiếp_nhận phân_tích yêu_cầu stakeholders business analysist teambackend engineer</t>
         </is>

</xml_diff>